<commit_message>
revise data, add javascript syntax for name selection
</commit_message>
<xml_diff>
--- a/AI_Website/project3Data.xlsx
+++ b/AI_Website/project3Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/AI_Website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbarron/Library/CloudStorage/OneDrive-UniversityofToronto/bootcamp/AITextDetector/AI_Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{4A7F2604-ED52-B24D-BAA9-D79196D44531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE83D591-8465-784D-A01A-9FCA3D34AFB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71132C6-8880-0B48-B34A-216E7D879C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12160" yWindow="500" windowWidth="16640" windowHeight="16440" xr2:uid="{73C40CA9-6724-264B-A24A-56B21B344AA0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="names" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4349,7 +4349,7 @@
   <dimension ref="A1:AK101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4478,7 +4478,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.XLOOKUP(D2,names!$G$2:$G$62,names!$H2:$H62)</f>
+        <f>_xlfn.XLOOKUP(D2,names!$G$2:$G$62,names!$H$2:$H$62)</f>
         <v>Leora Roakes</v>
       </c>
       <c r="F2">
@@ -4593,8 +4593,8 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f>_xlfn.XLOOKUP(D3,names!$G$2:$G$62,names!$H3:$H63)</f>
-        <v>Remus Duignan</v>
+        <f>_xlfn.XLOOKUP(D3,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Lula Furzey</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4708,8 +4708,8 @@
         <v>3</v>
       </c>
       <c r="E4" t="str">
-        <f>_xlfn.XLOOKUP(D4,names!$G$2:$G$62,names!$H4:$H64)</f>
-        <v>Kerstin Brookesbie</v>
+        <f>_xlfn.XLOOKUP(D4,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Remus Duignan</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -4823,8 +4823,8 @@
         <v>4</v>
       </c>
       <c r="E5" t="str">
-        <f>_xlfn.XLOOKUP(D5,names!$G$2:$G$62,names!$H5:$H65)</f>
-        <v>Sigmund Trounson</v>
+        <f>_xlfn.XLOOKUP(D5,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Teresita Laguerre</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -4938,8 +4938,8 @@
         <v>5</v>
       </c>
       <c r="E6" t="str">
-        <f>_xlfn.XLOOKUP(D6,names!$G$2:$G$62,names!$H6:$H66)</f>
-        <v>Bancroft Houseago</v>
+        <f>_xlfn.XLOOKUP(D6,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kerstin Brookesbie</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -5053,8 +5053,8 @@
         <v>6</v>
       </c>
       <c r="E7" t="str">
-        <f>_xlfn.XLOOKUP(D7,names!$G$2:$G$62,names!$H7:$H67)</f>
-        <v>Kristos Bakhrushin</v>
+        <f>_xlfn.XLOOKUP(D7,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Fulton Turbayne</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -5168,8 +5168,8 @@
         <v>7</v>
       </c>
       <c r="E8" t="str">
-        <f>_xlfn.XLOOKUP(D8,names!$G$2:$G$62,names!$H8:$H68)</f>
-        <v>Zonda Mellmoth</v>
+        <f>_xlfn.XLOOKUP(D8,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Sigmund Trounson</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -5283,8 +5283,8 @@
         <v>8</v>
       </c>
       <c r="E9" t="str">
-        <f>_xlfn.XLOOKUP(D9,names!$G$2:$G$62,names!$H9:$H69)</f>
-        <v>Delcina Hall-Gough</v>
+        <f>_xlfn.XLOOKUP(D9,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Ania Merali</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -5398,8 +5398,8 @@
         <v>9</v>
       </c>
       <c r="E10" t="str">
-        <f>_xlfn.XLOOKUP(D10,names!$G$2:$G$62,names!$H10:$H70)</f>
-        <v>Gustavo Collister</v>
+        <f>_xlfn.XLOOKUP(D10,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Bancroft Houseago</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -5513,8 +5513,8 @@
         <v>10</v>
       </c>
       <c r="E11" t="str">
-        <f>_xlfn.XLOOKUP(D11,names!$G$2:$G$62,names!$H11:$H71)</f>
-        <v>Gracia Adamov</v>
+        <f>_xlfn.XLOOKUP(D11,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Allissa MacNab</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -5628,8 +5628,8 @@
         <v>11</v>
       </c>
       <c r="E12" t="str">
-        <f>_xlfn.XLOOKUP(D12,names!$G$2:$G$62,names!$H12:$H72)</f>
-        <v>Hurley Danser</v>
+        <f>_xlfn.XLOOKUP(D12,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kristos Bakhrushin</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -5743,8 +5743,8 @@
         <v>12</v>
       </c>
       <c r="E13" t="str">
-        <f>_xlfn.XLOOKUP(D13,names!$G$2:$G$62,names!$H13:$H73)</f>
-        <v>Beaufort Hebbron</v>
+        <f>_xlfn.XLOOKUP(D13,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Alyson Daventry</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -5858,8 +5858,8 @@
         <v>13</v>
       </c>
       <c r="E14" t="str">
-        <f>_xlfn.XLOOKUP(D14,names!$G$2:$G$62,names!$H14:$H74)</f>
-        <v>Magdalena Coite</v>
+        <f>_xlfn.XLOOKUP(D14,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Zonda Mellmoth</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -5973,8 +5973,8 @@
         <v>14</v>
       </c>
       <c r="E15" t="str">
-        <f>_xlfn.XLOOKUP(D15,names!$G$2:$G$62,names!$H15:$H75)</f>
-        <v>Hetti Finnick</v>
+        <f>_xlfn.XLOOKUP(D15,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>De witt Bowick</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -6088,8 +6088,8 @@
         <v>15</v>
       </c>
       <c r="E16" t="str">
-        <f>_xlfn.XLOOKUP(D16,names!$G$2:$G$62,names!$H16:$H76)</f>
-        <v>Harlie Titcombe</v>
+        <f>_xlfn.XLOOKUP(D16,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Delcina Hall-Gough</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -6203,8 +6203,8 @@
         <v>16</v>
       </c>
       <c r="E17" t="str">
-        <f>_xlfn.XLOOKUP(D17,names!$G$2:$G$62,names!$H17:$H77)</f>
-        <v>Cullen Revell</v>
+        <f>_xlfn.XLOOKUP(D17,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Janie Gyford</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -6318,8 +6318,8 @@
         <v>17</v>
       </c>
       <c r="E18" t="str">
-        <f>_xlfn.XLOOKUP(D18,names!$G$2:$G$62,names!$H18:$H78)</f>
-        <v>Amabelle Wofenden</v>
+        <f>_xlfn.XLOOKUP(D18,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Gustavo Collister</v>
       </c>
       <c r="F18">
         <v>4</v>
@@ -6433,8 +6433,8 @@
         <v>1</v>
       </c>
       <c r="E19" t="str">
-        <f>_xlfn.XLOOKUP(D19,names!$G$2:$G$62,names!$H19:$H79)</f>
-        <v>Jeannette Riba</v>
+        <f>_xlfn.XLOOKUP(D19,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Leora Roakes</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -6548,8 +6548,8 @@
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <f>_xlfn.XLOOKUP(D20,names!$G$2:$G$62,names!$H20:$H80)</f>
-        <v>Dyanna Nesbeth</v>
+        <f>_xlfn.XLOOKUP(D20,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Lula Furzey</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -6663,8 +6663,8 @@
         <v>3</v>
       </c>
       <c r="E21" t="str">
-        <f>_xlfn.XLOOKUP(D21,names!$G$2:$G$62,names!$H21:$H81)</f>
-        <v>Mariel Pletts</v>
+        <f>_xlfn.XLOOKUP(D21,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Remus Duignan</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -6778,8 +6778,8 @@
         <v>4</v>
       </c>
       <c r="E22" t="str">
-        <f>_xlfn.XLOOKUP(D22,names!$G$2:$G$62,names!$H22:$H82)</f>
-        <v>Alexia Byres</v>
+        <f>_xlfn.XLOOKUP(D22,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Teresita Laguerre</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -6893,8 +6893,8 @@
         <v>5</v>
       </c>
       <c r="E23" t="str">
-        <f>_xlfn.XLOOKUP(D23,names!$G$2:$G$62,names!$H23:$H83)</f>
-        <v>Chrissie Helm</v>
+        <f>_xlfn.XLOOKUP(D23,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kerstin Brookesbie</v>
       </c>
       <c r="F23">
         <v>2</v>
@@ -7008,8 +7008,8 @@
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f>_xlfn.XLOOKUP(D24,names!$G$2:$G$62,names!$H24:$H84)</f>
-        <v>Uriah Postle</v>
+        <f>_xlfn.XLOOKUP(D24,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Fulton Turbayne</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -7123,8 +7123,8 @@
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f>_xlfn.XLOOKUP(D25,names!$G$2:$G$62,names!$H25:$H85)</f>
-        <v>Ilysa Sanja</v>
+        <f>_xlfn.XLOOKUP(D25,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Sigmund Trounson</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -7238,8 +7238,8 @@
         <v>8</v>
       </c>
       <c r="E26" t="str">
-        <f>_xlfn.XLOOKUP(D26,names!$G$2:$G$62,names!$H26:$H86)</f>
-        <v>Kippy Dewdeny</v>
+        <f>_xlfn.XLOOKUP(D26,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Ania Merali</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -7353,8 +7353,8 @@
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f>_xlfn.XLOOKUP(D27,names!$G$2:$G$62,names!$H27:$H87)</f>
-        <v>Noland Back</v>
+        <f>_xlfn.XLOOKUP(D27,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Bancroft Houseago</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -7468,8 +7468,8 @@
         <v>10</v>
       </c>
       <c r="E28" t="str">
-        <f>_xlfn.XLOOKUP(D28,names!$G$2:$G$62,names!$H28:$H88)</f>
-        <v>Flossie Whelband</v>
+        <f>_xlfn.XLOOKUP(D28,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Allissa MacNab</v>
       </c>
       <c r="F28">
         <v>3</v>
@@ -7583,8 +7583,8 @@
         <v>11</v>
       </c>
       <c r="E29" t="str">
-        <f>_xlfn.XLOOKUP(D29,names!$G$2:$G$62,names!$H29:$H89)</f>
-        <v>Belvia Chiene</v>
+        <f>_xlfn.XLOOKUP(D29,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kristos Bakhrushin</v>
       </c>
       <c r="F29">
         <v>3</v>
@@ -7698,8 +7698,8 @@
         <v>12</v>
       </c>
       <c r="E30" t="str">
-        <f>_xlfn.XLOOKUP(D30,names!$G$2:$G$62,names!$H30:$H90)</f>
-        <v>Ranna Beldon</v>
+        <f>_xlfn.XLOOKUP(D30,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Alyson Daventry</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -7813,8 +7813,8 @@
         <v>13</v>
       </c>
       <c r="E31" t="str">
-        <f>_xlfn.XLOOKUP(D31,names!$G$2:$G$62,names!$H31:$H91)</f>
-        <v>Marc Havvock</v>
+        <f>_xlfn.XLOOKUP(D31,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Zonda Mellmoth</v>
       </c>
       <c r="F31">
         <v>4</v>
@@ -7928,8 +7928,8 @@
         <v>14</v>
       </c>
       <c r="E32" t="str">
-        <f>_xlfn.XLOOKUP(D32,names!$G$2:$G$62,names!$H32:$H92)</f>
-        <v>Cori Kingswell</v>
+        <f>_xlfn.XLOOKUP(D32,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>De witt Bowick</v>
       </c>
       <c r="F32">
         <v>4</v>
@@ -8043,8 +8043,8 @@
         <v>15</v>
       </c>
       <c r="E33" t="str">
-        <f>_xlfn.XLOOKUP(D33,names!$G$2:$G$62,names!$H33:$H93)</f>
-        <v>Lutero Whiskerd</v>
+        <f>_xlfn.XLOOKUP(D33,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Delcina Hall-Gough</v>
       </c>
       <c r="F33">
         <v>4</v>
@@ -8158,8 +8158,8 @@
         <v>16</v>
       </c>
       <c r="E34" t="str">
-        <f>_xlfn.XLOOKUP(D34,names!$G$2:$G$62,names!$H34:$H94)</f>
-        <v>Elwira Pentycost</v>
+        <f>_xlfn.XLOOKUP(D34,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Janie Gyford</v>
       </c>
       <c r="F34">
         <v>4</v>
@@ -8273,8 +8273,8 @@
         <v>17</v>
       </c>
       <c r="E35" t="str">
-        <f>_xlfn.XLOOKUP(D35,names!$G$2:$G$62,names!$H35:$H95)</f>
-        <v>Birdie Sporton</v>
+        <f>_xlfn.XLOOKUP(D35,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Gustavo Collister</v>
       </c>
       <c r="F35">
         <v>4</v>
@@ -8388,8 +8388,8 @@
         <v>1</v>
       </c>
       <c r="E36" t="str">
-        <f>_xlfn.XLOOKUP(D36,names!$G$2:$G$62,names!$H36:$H96)</f>
-        <v>Rodina Fawke</v>
+        <f>_xlfn.XLOOKUP(D36,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Leora Roakes</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -8503,8 +8503,8 @@
         <v>2</v>
       </c>
       <c r="E37" t="str">
-        <f>_xlfn.XLOOKUP(D37,names!$G$2:$G$62,names!$H37:$H97)</f>
-        <v>Tara Petel</v>
+        <f>_xlfn.XLOOKUP(D37,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Lula Furzey</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -8618,8 +8618,8 @@
         <v>3</v>
       </c>
       <c r="E38" t="str">
-        <f>_xlfn.XLOOKUP(D38,names!$G$2:$G$62,names!$H38:$H98)</f>
-        <v>Rosaleen O'Tierney</v>
+        <f>_xlfn.XLOOKUP(D38,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Remus Duignan</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -8733,8 +8733,8 @@
         <v>4</v>
       </c>
       <c r="E39" t="str">
-        <f>_xlfn.XLOOKUP(D39,names!$G$2:$G$62,names!$H39:$H99)</f>
-        <v>Pennie Slavin</v>
+        <f>_xlfn.XLOOKUP(D39,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Teresita Laguerre</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -8848,8 +8848,8 @@
         <v>5</v>
       </c>
       <c r="E40" t="str">
-        <f>_xlfn.XLOOKUP(D40,names!$G$2:$G$62,names!$H40:$H100)</f>
-        <v>Gherardo Ride</v>
+        <f>_xlfn.XLOOKUP(D40,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kerstin Brookesbie</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -8963,8 +8963,8 @@
         <v>6</v>
       </c>
       <c r="E41" t="str">
-        <f>_xlfn.XLOOKUP(D41,names!$G$2:$G$62,names!$H41:$H101)</f>
-        <v>Missie Winsom</v>
+        <f>_xlfn.XLOOKUP(D41,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Fulton Turbayne</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -9078,8 +9078,8 @@
         <v>7</v>
       </c>
       <c r="E42" t="str">
-        <f>_xlfn.XLOOKUP(D42,names!$G$2:$G$62,names!$H42:$H102)</f>
-        <v>Anneliese Tod</v>
+        <f>_xlfn.XLOOKUP(D42,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Sigmund Trounson</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -9193,8 +9193,8 @@
         <v>8</v>
       </c>
       <c r="E43" t="str">
-        <f>_xlfn.XLOOKUP(D43,names!$G$2:$G$62,names!$H43:$H103)</f>
-        <v>Jeana Glanvill</v>
+        <f>_xlfn.XLOOKUP(D43,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Ania Merali</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -9308,8 +9308,8 @@
         <v>9</v>
       </c>
       <c r="E44" t="str">
-        <f>_xlfn.XLOOKUP(D44,names!$G$2:$G$62,names!$H44:$H104)</f>
-        <v>Orin Van de Vlies</v>
+        <f>_xlfn.XLOOKUP(D44,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Bancroft Houseago</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -9423,8 +9423,8 @@
         <v>10</v>
       </c>
       <c r="E45" t="str">
-        <f>_xlfn.XLOOKUP(D45,names!$G$2:$G$62,names!$H45:$H105)</f>
-        <v>Bing Forber</v>
+        <f>_xlfn.XLOOKUP(D45,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Allissa MacNab</v>
       </c>
       <c r="F45">
         <v>3</v>
@@ -9538,8 +9538,8 @@
         <v>11</v>
       </c>
       <c r="E46" t="str">
-        <f>_xlfn.XLOOKUP(D46,names!$G$2:$G$62,names!$H46:$H106)</f>
-        <v>Maryrose Neath</v>
+        <f>_xlfn.XLOOKUP(D46,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kristos Bakhrushin</v>
       </c>
       <c r="F46">
         <v>3</v>
@@ -9653,8 +9653,8 @@
         <v>12</v>
       </c>
       <c r="E47" t="str">
-        <f>_xlfn.XLOOKUP(D47,names!$G$2:$G$62,names!$H47:$H107)</f>
-        <v>Daloris Grennan</v>
+        <f>_xlfn.XLOOKUP(D47,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Alyson Daventry</v>
       </c>
       <c r="F47">
         <v>3</v>
@@ -9768,8 +9768,8 @@
         <v>13</v>
       </c>
       <c r="E48" t="str">
-        <f>_xlfn.XLOOKUP(D48,names!$G$2:$G$62,names!$H48:$H108)</f>
-        <v>Rayshell Skellen</v>
+        <f>_xlfn.XLOOKUP(D48,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Zonda Mellmoth</v>
       </c>
       <c r="F48">
         <v>4</v>
@@ -9883,8 +9883,8 @@
         <v>14</v>
       </c>
       <c r="E49" t="str">
-        <f>_xlfn.XLOOKUP(D49,names!$G$2:$G$62,names!$H49:$H109)</f>
-        <v>Angel Bedells</v>
+        <f>_xlfn.XLOOKUP(D49,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>De witt Bowick</v>
       </c>
       <c r="F49">
         <v>4</v>
@@ -9997,9 +9997,9 @@
       <c r="D50">
         <v>15</v>
       </c>
-      <c r="E50">
-        <f>_xlfn.XLOOKUP(D50,names!$G$2:$G$62,names!$H50:$H110)</f>
-        <v>0</v>
+      <c r="E50" t="str">
+        <f>_xlfn.XLOOKUP(D50,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Delcina Hall-Gough</v>
       </c>
       <c r="F50">
         <v>4</v>
@@ -10112,9 +10112,9 @@
       <c r="D51">
         <v>16</v>
       </c>
-      <c r="E51">
-        <f>_xlfn.XLOOKUP(D51,names!$G$2:$G$62,names!$H51:$H111)</f>
-        <v>0</v>
+      <c r="E51" t="str">
+        <f>_xlfn.XLOOKUP(D51,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Janie Gyford</v>
       </c>
       <c r="F51">
         <v>4</v>
@@ -10227,9 +10227,9 @@
       <c r="D52">
         <v>17</v>
       </c>
-      <c r="E52">
-        <f>_xlfn.XLOOKUP(D52,names!$G$2:$G$62,names!$H52:$H112)</f>
-        <v>0</v>
+      <c r="E52" t="str">
+        <f>_xlfn.XLOOKUP(D52,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Gustavo Collister</v>
       </c>
       <c r="F52">
         <v>4</v>
@@ -10343,8 +10343,8 @@
         <v>1</v>
       </c>
       <c r="E53" t="str">
-        <f>_xlfn.XLOOKUP(D53,names!$G$2:$G$62,names!$H53:$H113)</f>
-        <v>Eb Norker</v>
+        <f>_xlfn.XLOOKUP(D53,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Leora Roakes</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -10458,8 +10458,8 @@
         <v>2</v>
       </c>
       <c r="E54" t="str">
-        <f>_xlfn.XLOOKUP(D54,names!$G$2:$G$62,names!$H54:$H114)</f>
-        <v>Salomi Eisenberg</v>
+        <f>_xlfn.XLOOKUP(D54,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Lula Furzey</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -10573,8 +10573,8 @@
         <v>3</v>
       </c>
       <c r="E55" t="str">
-        <f>_xlfn.XLOOKUP(D55,names!$G$2:$G$62,names!$H55:$H115)</f>
-        <v>Adi Graber</v>
+        <f>_xlfn.XLOOKUP(D55,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Remus Duignan</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -10688,8 +10688,8 @@
         <v>4</v>
       </c>
       <c r="E56" t="str">
-        <f>_xlfn.XLOOKUP(D56,names!$G$2:$G$62,names!$H56:$H116)</f>
-        <v>Sonny Grimsdike</v>
+        <f>_xlfn.XLOOKUP(D56,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Teresita Laguerre</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -10803,8 +10803,8 @@
         <v>5</v>
       </c>
       <c r="E57" t="str">
-        <f>_xlfn.XLOOKUP(D57,names!$G$2:$G$62,names!$H57:$H117)</f>
-        <v>Fonzie Stonebridge</v>
+        <f>_xlfn.XLOOKUP(D57,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kerstin Brookesbie</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -10917,9 +10917,9 @@
       <c r="D58">
         <v>6</v>
       </c>
-      <c r="E58">
-        <f>_xlfn.XLOOKUP(D58,names!$G$2:$G$62,names!$H58:$H118)</f>
-        <v>0</v>
+      <c r="E58" t="str">
+        <f>_xlfn.XLOOKUP(D58,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Fulton Turbayne</v>
       </c>
       <c r="F58">
         <v>2</v>
@@ -11032,9 +11032,9 @@
       <c r="D59">
         <v>7</v>
       </c>
-      <c r="E59">
-        <f>_xlfn.XLOOKUP(D59,names!$G$2:$G$62,names!$H59:$H119)</f>
-        <v>0</v>
+      <c r="E59" t="str">
+        <f>_xlfn.XLOOKUP(D59,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Sigmund Trounson</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -11147,9 +11147,9 @@
       <c r="D60">
         <v>8</v>
       </c>
-      <c r="E60">
-        <f>_xlfn.XLOOKUP(D60,names!$G$2:$G$62,names!$H60:$H120)</f>
-        <v>0</v>
+      <c r="E60" t="str">
+        <f>_xlfn.XLOOKUP(D60,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Ania Merali</v>
       </c>
       <c r="F60">
         <v>2</v>
@@ -11262,9 +11262,9 @@
       <c r="D61">
         <v>9</v>
       </c>
-      <c r="E61">
-        <f>_xlfn.XLOOKUP(D61,names!$G$2:$G$62,names!$H61:$H121)</f>
-        <v>0</v>
+      <c r="E61" t="str">
+        <f>_xlfn.XLOOKUP(D61,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Bancroft Houseago</v>
       </c>
       <c r="F61">
         <v>3</v>
@@ -11377,9 +11377,9 @@
       <c r="D62">
         <v>10</v>
       </c>
-      <c r="E62">
-        <f>_xlfn.XLOOKUP(D62,names!$G$2:$G$62,names!$H62:$H122)</f>
-        <v>0</v>
+      <c r="E62" t="str">
+        <f>_xlfn.XLOOKUP(D62,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Allissa MacNab</v>
       </c>
       <c r="F62">
         <v>3</v>
@@ -11492,9 +11492,9 @@
       <c r="D63">
         <v>11</v>
       </c>
-      <c r="E63">
-        <f>_xlfn.XLOOKUP(D63,names!$G$2:$G$62,names!$H63:$H123)</f>
-        <v>0</v>
+      <c r="E63" t="str">
+        <f>_xlfn.XLOOKUP(D63,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kristos Bakhrushin</v>
       </c>
       <c r="F63">
         <v>3</v>
@@ -11607,9 +11607,9 @@
       <c r="D64">
         <v>12</v>
       </c>
-      <c r="E64">
-        <f>_xlfn.XLOOKUP(D64,names!$G$2:$G$62,names!$H64:$H124)</f>
-        <v>0</v>
+      <c r="E64" t="str">
+        <f>_xlfn.XLOOKUP(D64,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Alyson Daventry</v>
       </c>
       <c r="F64">
         <v>3</v>
@@ -11722,9 +11722,9 @@
       <c r="D65">
         <v>13</v>
       </c>
-      <c r="E65">
-        <f>_xlfn.XLOOKUP(D65,names!$G$2:$G$62,names!$H65:$H125)</f>
-        <v>0</v>
+      <c r="E65" t="str">
+        <f>_xlfn.XLOOKUP(D65,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Zonda Mellmoth</v>
       </c>
       <c r="F65">
         <v>4</v>
@@ -11837,9 +11837,9 @@
       <c r="D66">
         <v>14</v>
       </c>
-      <c r="E66">
-        <f>_xlfn.XLOOKUP(D66,names!$G$2:$G$62,names!$H66:$H126)</f>
-        <v>0</v>
+      <c r="E66" t="str">
+        <f>_xlfn.XLOOKUP(D66,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>De witt Bowick</v>
       </c>
       <c r="F66">
         <v>4</v>
@@ -11952,9 +11952,9 @@
       <c r="D67">
         <v>15</v>
       </c>
-      <c r="E67">
-        <f>_xlfn.XLOOKUP(D67,names!$G$2:$G$62,names!$H67:$H127)</f>
-        <v>0</v>
+      <c r="E67" t="str">
+        <f>_xlfn.XLOOKUP(D67,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Delcina Hall-Gough</v>
       </c>
       <c r="F67">
         <v>4</v>
@@ -12067,9 +12067,9 @@
       <c r="D68">
         <v>16</v>
       </c>
-      <c r="E68">
-        <f>_xlfn.XLOOKUP(D68,names!$G$2:$G$62,names!$H68:$H128)</f>
-        <v>0</v>
+      <c r="E68" t="str">
+        <f>_xlfn.XLOOKUP(D68,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Janie Gyford</v>
       </c>
       <c r="F68">
         <v>4</v>
@@ -12182,9 +12182,9 @@
       <c r="D69">
         <v>17</v>
       </c>
-      <c r="E69">
-        <f>_xlfn.XLOOKUP(D69,names!$G$2:$G$62,names!$H69:$H129)</f>
-        <v>0</v>
+      <c r="E69" t="str">
+        <f>_xlfn.XLOOKUP(D69,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Gustavo Collister</v>
       </c>
       <c r="F69">
         <v>4</v>
@@ -12297,9 +12297,9 @@
       <c r="D70">
         <v>1</v>
       </c>
-      <c r="E70">
-        <f>_xlfn.XLOOKUP(D70,names!$G$2:$G$62,names!$H70:$H130)</f>
-        <v>0</v>
+      <c r="E70" t="str">
+        <f>_xlfn.XLOOKUP(D70,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Leora Roakes</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -12412,9 +12412,9 @@
       <c r="D71">
         <v>2</v>
       </c>
-      <c r="E71">
-        <f>_xlfn.XLOOKUP(D71,names!$G$2:$G$62,names!$H71:$H131)</f>
-        <v>0</v>
+      <c r="E71" t="str">
+        <f>_xlfn.XLOOKUP(D71,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Lula Furzey</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -12527,9 +12527,9 @@
       <c r="D72">
         <v>3</v>
       </c>
-      <c r="E72">
-        <f>_xlfn.XLOOKUP(D72,names!$G$2:$G$62,names!$H72:$H132)</f>
-        <v>0</v>
+      <c r="E72" t="str">
+        <f>_xlfn.XLOOKUP(D72,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Remus Duignan</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -12642,9 +12642,9 @@
       <c r="D73">
         <v>4</v>
       </c>
-      <c r="E73">
-        <f>_xlfn.XLOOKUP(D73,names!$G$2:$G$62,names!$H73:$H133)</f>
-        <v>0</v>
+      <c r="E73" t="str">
+        <f>_xlfn.XLOOKUP(D73,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Teresita Laguerre</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -12757,9 +12757,9 @@
       <c r="D74">
         <v>5</v>
       </c>
-      <c r="E74">
-        <f>_xlfn.XLOOKUP(D74,names!$G$2:$G$62,names!$H74:$H134)</f>
-        <v>0</v>
+      <c r="E74" t="str">
+        <f>_xlfn.XLOOKUP(D74,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kerstin Brookesbie</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -12872,9 +12872,9 @@
       <c r="D75">
         <v>6</v>
       </c>
-      <c r="E75">
-        <f>_xlfn.XLOOKUP(D75,names!$G$2:$G$62,names!$H75:$H135)</f>
-        <v>0</v>
+      <c r="E75" t="str">
+        <f>_xlfn.XLOOKUP(D75,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Fulton Turbayne</v>
       </c>
       <c r="F75">
         <v>2</v>
@@ -12987,9 +12987,9 @@
       <c r="D76">
         <v>7</v>
       </c>
-      <c r="E76">
-        <f>_xlfn.XLOOKUP(D76,names!$G$2:$G$62,names!$H76:$H136)</f>
-        <v>0</v>
+      <c r="E76" t="str">
+        <f>_xlfn.XLOOKUP(D76,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Sigmund Trounson</v>
       </c>
       <c r="F76">
         <v>2</v>
@@ -13102,9 +13102,9 @@
       <c r="D77">
         <v>8</v>
       </c>
-      <c r="E77">
-        <f>_xlfn.XLOOKUP(D77,names!$G$2:$G$62,names!$H77:$H137)</f>
-        <v>0</v>
+      <c r="E77" t="str">
+        <f>_xlfn.XLOOKUP(D77,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Ania Merali</v>
       </c>
       <c r="F77">
         <v>2</v>
@@ -13217,9 +13217,9 @@
       <c r="D78">
         <v>9</v>
       </c>
-      <c r="E78">
-        <f>_xlfn.XLOOKUP(D78,names!$G$2:$G$62,names!$H78:$H138)</f>
-        <v>0</v>
+      <c r="E78" t="str">
+        <f>_xlfn.XLOOKUP(D78,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Bancroft Houseago</v>
       </c>
       <c r="F78">
         <v>3</v>
@@ -13332,9 +13332,9 @@
       <c r="D79">
         <v>10</v>
       </c>
-      <c r="E79">
-        <f>_xlfn.XLOOKUP(D79,names!$G$2:$G$62,names!$H79:$H139)</f>
-        <v>0</v>
+      <c r="E79" t="str">
+        <f>_xlfn.XLOOKUP(D79,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Allissa MacNab</v>
       </c>
       <c r="F79">
         <v>3</v>
@@ -13447,9 +13447,9 @@
       <c r="D80">
         <v>11</v>
       </c>
-      <c r="E80">
-        <f>_xlfn.XLOOKUP(D80,names!$G$2:$G$62,names!$H80:$H140)</f>
-        <v>0</v>
+      <c r="E80" t="str">
+        <f>_xlfn.XLOOKUP(D80,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kristos Bakhrushin</v>
       </c>
       <c r="F80">
         <v>3</v>
@@ -13562,9 +13562,9 @@
       <c r="D81">
         <v>12</v>
       </c>
-      <c r="E81">
-        <f>_xlfn.XLOOKUP(D81,names!$G$2:$G$62,names!$H81:$H141)</f>
-        <v>0</v>
+      <c r="E81" t="str">
+        <f>_xlfn.XLOOKUP(D81,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Alyson Daventry</v>
       </c>
       <c r="F81">
         <v>3</v>
@@ -13677,9 +13677,9 @@
       <c r="D82">
         <v>13</v>
       </c>
-      <c r="E82">
-        <f>_xlfn.XLOOKUP(D82,names!$G$2:$G$62,names!$H82:$H142)</f>
-        <v>0</v>
+      <c r="E82" t="str">
+        <f>_xlfn.XLOOKUP(D82,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Zonda Mellmoth</v>
       </c>
       <c r="F82">
         <v>4</v>
@@ -13792,9 +13792,9 @@
       <c r="D83">
         <v>14</v>
       </c>
-      <c r="E83">
-        <f>_xlfn.XLOOKUP(D83,names!$G$2:$G$62,names!$H83:$H143)</f>
-        <v>0</v>
+      <c r="E83" t="str">
+        <f>_xlfn.XLOOKUP(D83,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>De witt Bowick</v>
       </c>
       <c r="F83">
         <v>4</v>
@@ -13907,9 +13907,9 @@
       <c r="D84">
         <v>15</v>
       </c>
-      <c r="E84">
-        <f>_xlfn.XLOOKUP(D84,names!$G$2:$G$62,names!$H84:$H144)</f>
-        <v>0</v>
+      <c r="E84" t="str">
+        <f>_xlfn.XLOOKUP(D84,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Delcina Hall-Gough</v>
       </c>
       <c r="F84">
         <v>4</v>
@@ -14022,9 +14022,9 @@
       <c r="D85">
         <v>16</v>
       </c>
-      <c r="E85">
-        <f>_xlfn.XLOOKUP(D85,names!$G$2:$G$62,names!$H85:$H145)</f>
-        <v>0</v>
+      <c r="E85" t="str">
+        <f>_xlfn.XLOOKUP(D85,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Janie Gyford</v>
       </c>
       <c r="F85">
         <v>4</v>
@@ -14137,9 +14137,9 @@
       <c r="D86" s="2">
         <v>1</v>
       </c>
-      <c r="E86">
-        <f>_xlfn.XLOOKUP(D86,names!$G$2:$G$62,names!$H86:$H146)</f>
-        <v>0</v>
+      <c r="E86" t="str">
+        <f>_xlfn.XLOOKUP(D86,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Leora Roakes</v>
       </c>
       <c r="F86" s="2">
         <v>1</v>
@@ -14252,9 +14252,9 @@
       <c r="D87" s="2">
         <v>2</v>
       </c>
-      <c r="E87">
-        <f>_xlfn.XLOOKUP(D87,names!$G$2:$G$62,names!$H87:$H147)</f>
-        <v>0</v>
+      <c r="E87" t="str">
+        <f>_xlfn.XLOOKUP(D87,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Lula Furzey</v>
       </c>
       <c r="F87" s="2">
         <v>1</v>
@@ -14367,9 +14367,9 @@
       <c r="D88" s="2">
         <v>3</v>
       </c>
-      <c r="E88">
-        <f>_xlfn.XLOOKUP(D88,names!$G$2:$G$62,names!$H88:$H148)</f>
-        <v>0</v>
+      <c r="E88" t="str">
+        <f>_xlfn.XLOOKUP(D88,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Remus Duignan</v>
       </c>
       <c r="F88" s="2">
         <v>1</v>
@@ -14482,9 +14482,9 @@
       <c r="D89" s="2">
         <v>4</v>
       </c>
-      <c r="E89">
-        <f>_xlfn.XLOOKUP(D89,names!$G$2:$G$62,names!$H89:$H149)</f>
-        <v>0</v>
+      <c r="E89" t="str">
+        <f>_xlfn.XLOOKUP(D89,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Teresita Laguerre</v>
       </c>
       <c r="F89" s="2">
         <v>1</v>
@@ -14597,9 +14597,9 @@
       <c r="D90" s="2">
         <v>5</v>
       </c>
-      <c r="E90">
-        <f>_xlfn.XLOOKUP(D90,names!$G$2:$G$62,names!$H90:$H150)</f>
-        <v>0</v>
+      <c r="E90" t="str">
+        <f>_xlfn.XLOOKUP(D90,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kerstin Brookesbie</v>
       </c>
       <c r="F90" s="2">
         <v>2</v>
@@ -14712,9 +14712,9 @@
       <c r="D91" s="2">
         <v>6</v>
       </c>
-      <c r="E91">
-        <f>_xlfn.XLOOKUP(D91,names!$G$2:$G$62,names!$H91:$H151)</f>
-        <v>0</v>
+      <c r="E91" t="str">
+        <f>_xlfn.XLOOKUP(D91,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Fulton Turbayne</v>
       </c>
       <c r="F91" s="2">
         <v>2</v>
@@ -14827,9 +14827,9 @@
       <c r="D92" s="2">
         <v>7</v>
       </c>
-      <c r="E92">
-        <f>_xlfn.XLOOKUP(D92,names!$G$2:$G$62,names!$H92:$H152)</f>
-        <v>0</v>
+      <c r="E92" t="str">
+        <f>_xlfn.XLOOKUP(D92,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Sigmund Trounson</v>
       </c>
       <c r="F92" s="2">
         <v>2</v>
@@ -14942,9 +14942,9 @@
       <c r="D93" s="2">
         <v>8</v>
       </c>
-      <c r="E93">
-        <f>_xlfn.XLOOKUP(D93,names!$G$2:$G$62,names!$H93:$H153)</f>
-        <v>0</v>
+      <c r="E93" t="str">
+        <f>_xlfn.XLOOKUP(D93,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Ania Merali</v>
       </c>
       <c r="F93" s="2">
         <v>2</v>
@@ -15057,9 +15057,9 @@
       <c r="D94" s="2">
         <v>9</v>
       </c>
-      <c r="E94">
-        <f>_xlfn.XLOOKUP(D94,names!$G$2:$G$62,names!$H94:$H154)</f>
-        <v>0</v>
+      <c r="E94" t="str">
+        <f>_xlfn.XLOOKUP(D94,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Bancroft Houseago</v>
       </c>
       <c r="F94" s="2">
         <v>3</v>
@@ -15172,9 +15172,9 @@
       <c r="D95" s="2">
         <v>10</v>
       </c>
-      <c r="E95">
-        <f>_xlfn.XLOOKUP(D95,names!$G$2:$G$62,names!$H95:$H155)</f>
-        <v>0</v>
+      <c r="E95" t="str">
+        <f>_xlfn.XLOOKUP(D95,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Allissa MacNab</v>
       </c>
       <c r="F95" s="2">
         <v>3</v>
@@ -15287,9 +15287,9 @@
       <c r="D96" s="2">
         <v>11</v>
       </c>
-      <c r="E96">
-        <f>_xlfn.XLOOKUP(D96,names!$G$2:$G$62,names!$H96:$H156)</f>
-        <v>0</v>
+      <c r="E96" t="str">
+        <f>_xlfn.XLOOKUP(D96,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Kristos Bakhrushin</v>
       </c>
       <c r="F96" s="2">
         <v>3</v>
@@ -15402,9 +15402,9 @@
       <c r="D97" s="2">
         <v>12</v>
       </c>
-      <c r="E97">
-        <f>_xlfn.XLOOKUP(D97,names!$G$2:$G$62,names!$H97:$H157)</f>
-        <v>0</v>
+      <c r="E97" t="str">
+        <f>_xlfn.XLOOKUP(D97,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Alyson Daventry</v>
       </c>
       <c r="F97" s="2">
         <v>3</v>
@@ -15517,9 +15517,9 @@
       <c r="D98" s="2">
         <v>13</v>
       </c>
-      <c r="E98">
-        <f>_xlfn.XLOOKUP(D98,names!$G$2:$G$62,names!$H98:$H158)</f>
-        <v>0</v>
+      <c r="E98" t="str">
+        <f>_xlfn.XLOOKUP(D98,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Zonda Mellmoth</v>
       </c>
       <c r="F98" s="2">
         <v>4</v>
@@ -15632,9 +15632,9 @@
       <c r="D99" s="2">
         <v>14</v>
       </c>
-      <c r="E99">
-        <f>_xlfn.XLOOKUP(D99,names!$G$2:$G$62,names!$H99:$H159)</f>
-        <v>0</v>
+      <c r="E99" t="str">
+        <f>_xlfn.XLOOKUP(D99,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>De witt Bowick</v>
       </c>
       <c r="F99" s="2">
         <v>4</v>
@@ -15747,9 +15747,9 @@
       <c r="D100" s="2">
         <v>15</v>
       </c>
-      <c r="E100">
-        <f>_xlfn.XLOOKUP(D100,names!$G$2:$G$62,names!$H100:$H160)</f>
-        <v>0</v>
+      <c r="E100" t="str">
+        <f>_xlfn.XLOOKUP(D100,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Delcina Hall-Gough</v>
       </c>
       <c r="F100" s="2">
         <v>4</v>
@@ -15862,9 +15862,9 @@
       <c r="D101" s="2">
         <v>16</v>
       </c>
-      <c r="E101">
-        <f>_xlfn.XLOOKUP(D101,names!$G$2:$G$62,names!$H101:$H161)</f>
-        <v>0</v>
+      <c r="E101" t="str">
+        <f>_xlfn.XLOOKUP(D101,names!$G$2:$G$62,names!$H$2:$H$62)</f>
+        <v>Janie Gyford</v>
       </c>
       <c r="F101" s="2">
         <v>4</v>
@@ -15974,7 +15974,7 @@
   <dimension ref="A1:P133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>